<commit_message>
update to rac pump code
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github Repos\IS401\RAC\Agritech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197B1821-DC24-405C-8CE9-696C23A952BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618C37E8-295B-4518-B797-479714DA4796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{13700059-ED45-4C40-BE39-042EB1367643}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{13700059-ED45-4C40-BE39-042EB1367643}"/>
   </bookViews>
   <sheets>
     <sheet name="RAC Ver 1" sheetId="1" r:id="rId1"/>
     <sheet name="RAC Ver 2" sheetId="3" r:id="rId2"/>
+    <sheet name="RAC Ver 3" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="51">
   <si>
     <t>BOM</t>
   </si>
@@ -187,6 +188,9 @@
   </si>
   <si>
     <t>Roughly 5.00 Total</t>
+  </si>
+  <si>
+    <t>CO2 sensor</t>
   </si>
 </sst>
 </file>
@@ -231,12 +235,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -352,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -379,9 +389,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -874,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7EDE3F-947F-4A72-9FC4-8FC04454CACB}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1181,16 +1193,16 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="7" t="s">
         <v>47</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="D16" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16">
         <v>1</v>
       </c>
       <c r="F16" s="4">
@@ -1233,4 +1245,387 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D173D40-7B5C-4D73-A8EF-B3CDDBF054AF}">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.109375" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" customWidth="1"/>
+    <col min="6" max="6" width="16.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="13"/>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5" s="5">
+        <f t="shared" ref="F5:F18" si="0">IF(C5="USD",D5*E5*1.36,E5*D5)</f>
+        <v>38.700000000000003</v>
+      </c>
+      <c r="H5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
+        <f t="shared" si="0"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="13"/>
+      <c r="B7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5">
+        <f t="shared" si="0"/>
+        <v>53.720000000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="13"/>
+      <c r="B8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="9">
+        <f t="shared" ref="F8" si="1">IF(C8="USD",D8*E8*1.36,E8*D8)</f>
+        <v>108.66400000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="22"/>
+      <c r="B9" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="24">
+        <v>50</v>
+      </c>
+      <c r="E9" s="25">
+        <v>1</v>
+      </c>
+      <c r="F9" s="26">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="4">
+        <f>IF(C10="USD",D10*E10*1.36,E10*D10)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="5"/>
+      <c r="B11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="5">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="5"/>
+      <c r="B12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="9"/>
+      <c r="B13" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="3">
+        <v>7</v>
+      </c>
+      <c r="F14" s="4">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" s="5">
+        <f t="shared" si="0"/>
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1</v>
+      </c>
+      <c r="F16" s="4">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+      <c r="B17" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="9"/>
+      <c r="B18" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="8">
+        <v>1</v>
+      </c>
+      <c r="F18" s="4">
+        <f t="shared" si="0"/>
+        <v>9.51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E19" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="18">
+        <f>SUM(F3:F18)</f>
+        <v>371.39400000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>